<commit_message>
Replaced with real data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -136,6 +136,33 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Oslo Vest</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Nesodden</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Vet ikke</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Lillestrøm</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Nittedal</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Mindre enn 1 time</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">eidsvoll</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Åros</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">18-19 år</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">NORDMØRE</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -232,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P11" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:P11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P60" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:P60"/>
   <x:tableColumns count="16">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Starttidspunkt" dataDxfId="3"/>
@@ -1109,11 +1136,2363 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
+    <x:row r="12" hidden="0">
+      <x:c r="A12">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B12" s="2">
+        <x:v>44693.7467476852</x:v>
+      </x:c>
+      <x:c r="C12" s="2">
+        <x:v>44693.7474537037</x:v>
+      </x:c>
+      <x:c r="D12" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E12" s="10" t="s"/>
+      <x:c r="F12" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G12" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H12" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I12" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="J12" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K12" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L12" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M12" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N12" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O12" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P12" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" hidden="0">
+      <x:c r="A13">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B13" s="2">
+        <x:v>44693.7666666667</x:v>
+      </x:c>
+      <x:c r="C13" s="2">
+        <x:v>44693.7672685185</x:v>
+      </x:c>
+      <x:c r="D13" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E13" s="10" t="s"/>
+      <x:c r="F13" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G13" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H13" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I13" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J13" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K13" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L13" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M13" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N13" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O13" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="P13" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" hidden="0">
+      <x:c r="A14">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B14" s="2">
+        <x:v>44693.8320833333</x:v>
+      </x:c>
+      <x:c r="C14" s="2">
+        <x:v>44693.8323032407</x:v>
+      </x:c>
+      <x:c r="D14" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E14" s="10" t="s"/>
+      <x:c r="F14" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G14" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H14" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I14" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J14" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K14" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L14" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M14" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="N14" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="O14" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P14" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" hidden="0">
+      <x:c r="A15">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B15" s="2">
+        <x:v>44694.3433796296</x:v>
+      </x:c>
+      <x:c r="C15" s="2">
+        <x:v>44694.3442476852</x:v>
+      </x:c>
+      <x:c r="D15" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E15" s="10" t="s"/>
+      <x:c r="F15" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G15" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H15" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I15" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J15" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K15" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L15" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M15" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N15" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O15" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P15" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" hidden="0">
+      <x:c r="A16">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B16" s="2">
+        <x:v>44694.3456134259</x:v>
+      </x:c>
+      <x:c r="C16" s="2">
+        <x:v>44694.3461921296</x:v>
+      </x:c>
+      <x:c r="D16" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E16" s="10" t="s"/>
+      <x:c r="F16" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G16" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H16" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I16" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J16" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K16" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L16" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M16" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N16" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O16" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P16" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" hidden="0">
+      <x:c r="A17">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B17" s="2">
+        <x:v>44694.3675925926</x:v>
+      </x:c>
+      <x:c r="C17" s="2">
+        <x:v>44694.3683796296</x:v>
+      </x:c>
+      <x:c r="D17" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E17" s="10" t="s"/>
+      <x:c r="F17" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G17" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H17" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I17" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J17" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K17" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L17" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M17" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N17" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O17" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="P17" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" hidden="0">
+      <x:c r="A18">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B18" s="2">
+        <x:v>44694.3681597222</x:v>
+      </x:c>
+      <x:c r="C18" s="2">
+        <x:v>44694.3691898148</x:v>
+      </x:c>
+      <x:c r="D18" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E18" s="10" t="s"/>
+      <x:c r="F18" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G18" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H18" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I18" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="J18" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K18" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L18" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M18" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N18" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O18" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P18" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" hidden="0">
+      <x:c r="A19">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B19" s="2">
+        <x:v>44694.3681481481</x:v>
+      </x:c>
+      <x:c r="C19" s="2">
+        <x:v>44694.3693634259</x:v>
+      </x:c>
+      <x:c r="D19" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E19" s="10" t="s"/>
+      <x:c r="F19" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G19" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H19" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I19" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J19" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K19" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L19" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M19" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N19" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O19" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P19" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" hidden="0">
+      <x:c r="A20">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B20" s="2">
+        <x:v>44694.3691435185</x:v>
+      </x:c>
+      <x:c r="C20" s="2">
+        <x:v>44694.3698032407</x:v>
+      </x:c>
+      <x:c r="D20" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E20" s="10" t="s"/>
+      <x:c r="F20" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G20" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H20" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I20" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="J20" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K20" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L20" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M20" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="N20" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="O20" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="P20" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" hidden="0">
+      <x:c r="A21">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B21" s="2">
+        <x:v>44694.3703819444</x:v>
+      </x:c>
+      <x:c r="C21" s="2">
+        <x:v>44694.3710763889</x:v>
+      </x:c>
+      <x:c r="D21" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E21" s="10" t="s"/>
+      <x:c r="F21" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G21" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H21" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I21" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="J21" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K21" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L21" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M21" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N21" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O21" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P21" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" hidden="0">
+      <x:c r="A22">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B22" s="2">
+        <x:v>44694.3725694444</x:v>
+      </x:c>
+      <x:c r="C22" s="2">
+        <x:v>44694.3731944444</x:v>
+      </x:c>
+      <x:c r="D22" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E22" s="10" t="s"/>
+      <x:c r="F22" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G22" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H22" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I22" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J22" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K22" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L22" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M22" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="N22" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O22" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P22" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" hidden="0">
+      <x:c r="A23">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B23" s="2">
+        <x:v>44694.3722222222</x:v>
+      </x:c>
+      <x:c r="C23" s="2">
+        <x:v>44694.373287037</x:v>
+      </x:c>
+      <x:c r="D23" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E23" s="10" t="s"/>
+      <x:c r="F23" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G23" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H23" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I23" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="J23" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K23" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L23" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M23" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N23" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O23" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P23" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" hidden="0">
+      <x:c r="A24">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B24" s="2">
+        <x:v>44694.3742939815</x:v>
+      </x:c>
+      <x:c r="C24" s="2">
+        <x:v>44694.3747685185</x:v>
+      </x:c>
+      <x:c r="D24" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E24" s="10" t="s"/>
+      <x:c r="F24" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G24" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H24" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I24" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J24" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K24" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L24" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M24" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N24" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O24" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P24" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" hidden="0">
+      <x:c r="A25">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B25" s="2">
+        <x:v>44694.3772453704</x:v>
+      </x:c>
+      <x:c r="C25" s="2">
+        <x:v>44694.3776273148</x:v>
+      </x:c>
+      <x:c r="D25" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E25" s="10" t="s"/>
+      <x:c r="F25" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G25" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H25" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I25" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="J25" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K25" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L25" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M25" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N25" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O25" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P25" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" hidden="0">
+      <x:c r="A26">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B26" s="2">
+        <x:v>44694.3761805556</x:v>
+      </x:c>
+      <x:c r="C26" s="2">
+        <x:v>44694.3777083333</x:v>
+      </x:c>
+      <x:c r="D26" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E26" s="10" t="s"/>
+      <x:c r="F26" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G26" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H26" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I26" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J26" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K26" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L26" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M26" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N26" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O26" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P26" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" hidden="0">
+      <x:c r="A27">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B27" s="2">
+        <x:v>44694.3767476852</x:v>
+      </x:c>
+      <x:c r="C27" s="2">
+        <x:v>44694.3777314815</x:v>
+      </x:c>
+      <x:c r="D27" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E27" s="10" t="s"/>
+      <x:c r="F27" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G27" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H27" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I27" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J27" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K27" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L27" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M27" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N27" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O27" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P27" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" hidden="0">
+      <x:c r="A28">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B28" s="2">
+        <x:v>44694.3776967593</x:v>
+      </x:c>
+      <x:c r="C28" s="2">
+        <x:v>44694.3785416667</x:v>
+      </x:c>
+      <x:c r="D28" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E28" s="10" t="s"/>
+      <x:c r="F28" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G28" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H28" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I28" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J28" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K28" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L28" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M28" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N28" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O28" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P28" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" hidden="0">
+      <x:c r="A29">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B29" s="2">
+        <x:v>44694.3779861111</x:v>
+      </x:c>
+      <x:c r="C29" s="2">
+        <x:v>44694.3793171296</x:v>
+      </x:c>
+      <x:c r="D29" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E29" s="10" t="s"/>
+      <x:c r="F29" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G29" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H29" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I29" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J29" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K29" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L29" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M29" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N29" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O29" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="P29" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" hidden="0">
+      <x:c r="A30">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B30" s="2">
+        <x:v>44694.3791666667</x:v>
+      </x:c>
+      <x:c r="C30" s="2">
+        <x:v>44694.3799074074</x:v>
+      </x:c>
+      <x:c r="D30" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E30" s="10" t="s"/>
+      <x:c r="F30" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G30" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H30" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I30" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="J30" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K30" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L30" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M30" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N30" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O30" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P30" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" hidden="0">
+      <x:c r="A31">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B31" s="2">
+        <x:v>44694.3791435185</x:v>
+      </x:c>
+      <x:c r="C31" s="2">
+        <x:v>44694.3803587963</x:v>
+      </x:c>
+      <x:c r="D31" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E31" s="10" t="s"/>
+      <x:c r="F31" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G31" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H31" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I31" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J31" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K31" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L31" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M31" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N31" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O31" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="P31" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" hidden="0">
+      <x:c r="A32">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B32" s="2">
+        <x:v>44694.3810185185</x:v>
+      </x:c>
+      <x:c r="C32" s="2">
+        <x:v>44694.3821527778</x:v>
+      </x:c>
+      <x:c r="D32" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E32" s="10" t="s"/>
+      <x:c r="F32" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G32" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H32" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I32" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J32" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K32" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L32" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M32" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N32" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O32" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P32" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" hidden="0">
+      <x:c r="A33">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B33" s="2">
+        <x:v>44694.3817476852</x:v>
+      </x:c>
+      <x:c r="C33" s="2">
+        <x:v>44694.3824421296</x:v>
+      </x:c>
+      <x:c r="D33" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E33" s="10" t="s"/>
+      <x:c r="F33" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G33" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H33" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I33" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J33" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K33" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L33" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M33" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N33" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O33" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P33" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" hidden="0">
+      <x:c r="A34">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B34" s="2">
+        <x:v>44694.3821296296</x:v>
+      </x:c>
+      <x:c r="C34" s="2">
+        <x:v>44694.3825694444</x:v>
+      </x:c>
+      <x:c r="D34" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E34" s="10" t="s"/>
+      <x:c r="F34" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G34" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H34" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I34" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J34" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K34" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L34" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M34" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N34" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O34" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P34" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" hidden="0">
+      <x:c r="A35">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B35" s="2">
+        <x:v>44694.3821180556</x:v>
+      </x:c>
+      <x:c r="C35" s="2">
+        <x:v>44694.3826967593</x:v>
+      </x:c>
+      <x:c r="D35" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E35" s="10" t="s"/>
+      <x:c r="F35" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G35" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H35" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I35" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J35" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K35" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L35" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M35" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N35" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O35" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P35" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" hidden="0">
+      <x:c r="A36">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B36" s="2">
+        <x:v>44694.3819444444</x:v>
+      </x:c>
+      <x:c r="C36" s="2">
+        <x:v>44694.3832175926</x:v>
+      </x:c>
+      <x:c r="D36" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E36" s="10" t="s"/>
+      <x:c r="F36" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G36" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H36" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I36" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J36" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K36" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L36" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M36" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N36" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O36" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P36" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" hidden="0">
+      <x:c r="A37">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B37" s="2">
+        <x:v>44694.3829166667</x:v>
+      </x:c>
+      <x:c r="C37" s="2">
+        <x:v>44694.3837384259</x:v>
+      </x:c>
+      <x:c r="D37" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E37" s="10" t="s"/>
+      <x:c r="F37" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G37" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H37" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I37" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J37" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K37" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L37" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M37" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N37" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="O37" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="P37" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" hidden="0">
+      <x:c r="A38">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B38" s="2">
+        <x:v>44694.3869328704</x:v>
+      </x:c>
+      <x:c r="C38" s="2">
+        <x:v>44694.3872685185</x:v>
+      </x:c>
+      <x:c r="D38" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E38" s="10" t="s"/>
+      <x:c r="F38" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G38" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H38" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I38" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J38" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K38" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L38" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M38" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N38" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O38" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P38" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" hidden="0">
+      <x:c r="A39">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B39" s="2">
+        <x:v>44694.387662037</x:v>
+      </x:c>
+      <x:c r="C39" s="2">
+        <x:v>44694.3881944444</x:v>
+      </x:c>
+      <x:c r="D39" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E39" s="10" t="s"/>
+      <x:c r="F39" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G39" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H39" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I39" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="J39" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K39" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L39" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M39" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N39" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O39" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P39" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" hidden="0">
+      <x:c r="A40">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B40" s="2">
+        <x:v>44694.3958564815</x:v>
+      </x:c>
+      <x:c r="C40" s="2">
+        <x:v>44694.3964930556</x:v>
+      </x:c>
+      <x:c r="D40" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E40" s="10" t="s"/>
+      <x:c r="F40" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G40" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H40" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I40" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J40" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K40" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L40" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M40" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N40" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O40" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P40" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" hidden="0">
+      <x:c r="A41">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B41" s="2">
+        <x:v>44694.4061805556</x:v>
+      </x:c>
+      <x:c r="C41" s="2">
+        <x:v>44694.4070138889</x:v>
+      </x:c>
+      <x:c r="D41" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E41" s="10" t="s"/>
+      <x:c r="F41" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G41" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H41" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I41" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J41" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K41" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L41" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M41" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N41" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O41" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P41" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" hidden="0">
+      <x:c r="A42">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B42" s="2">
+        <x:v>44694.4230092593</x:v>
+      </x:c>
+      <x:c r="C42" s="2">
+        <x:v>44694.4236111111</x:v>
+      </x:c>
+      <x:c r="D42" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E42" s="10" t="s"/>
+      <x:c r="F42" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G42" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H42" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I42" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J42" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K42" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L42" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M42" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="N42" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O42" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P42" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" hidden="0">
+      <x:c r="A43">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B43" s="2">
+        <x:v>44694.4265740741</x:v>
+      </x:c>
+      <x:c r="C43" s="2">
+        <x:v>44694.4270717593</x:v>
+      </x:c>
+      <x:c r="D43" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E43" s="10" t="s"/>
+      <x:c r="F43" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G43" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H43" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I43" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J43" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K43" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L43" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M43" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N43" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O43" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="P43" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" hidden="0">
+      <x:c r="A44">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B44" s="2">
+        <x:v>44694.4480439815</x:v>
+      </x:c>
+      <x:c r="C44" s="2">
+        <x:v>44694.4487037037</x:v>
+      </x:c>
+      <x:c r="D44" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E44" s="10" t="s"/>
+      <x:c r="F44" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G44" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H44" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I44" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J44" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K44" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L44" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M44" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="N44" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="O44" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P44" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" hidden="0">
+      <x:c r="A45">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B45" s="2">
+        <x:v>44694.4503356481</x:v>
+      </x:c>
+      <x:c r="C45" s="2">
+        <x:v>44694.4510069444</x:v>
+      </x:c>
+      <x:c r="D45" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E45" s="10" t="s"/>
+      <x:c r="F45" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G45" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H45" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I45" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J45" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K45" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L45" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M45" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="N45" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="O45" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="P45" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" hidden="0">
+      <x:c r="A46">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B46" s="2">
+        <x:v>44694.469537037</x:v>
+      </x:c>
+      <x:c r="C46" s="2">
+        <x:v>44694.4703703704</x:v>
+      </x:c>
+      <x:c r="D46" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E46" s="10" t="s"/>
+      <x:c r="F46" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G46" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H46" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I46" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J46" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K46" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L46" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M46" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N46" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="O46" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P46" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" hidden="0">
+      <x:c r="A47">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B47" s="2">
+        <x:v>44694.5293402778</x:v>
+      </x:c>
+      <x:c r="C47" s="2">
+        <x:v>44694.5312847222</x:v>
+      </x:c>
+      <x:c r="D47" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E47" s="10" t="s"/>
+      <x:c r="F47" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G47" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H47" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I47" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J47" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K47" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L47" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M47" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="N47" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O47" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P47" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" hidden="0">
+      <x:c r="A48">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B48" s="2">
+        <x:v>44694.5511458333</x:v>
+      </x:c>
+      <x:c r="C48" s="2">
+        <x:v>44694.551712963</x:v>
+      </x:c>
+      <x:c r="D48" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E48" s="10" t="s"/>
+      <x:c r="F48" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G48" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H48" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I48" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J48" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K48" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L48" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M48" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="N48" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O48" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="P48" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" hidden="0">
+      <x:c r="A49">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B49" s="2">
+        <x:v>44694.5597337963</x:v>
+      </x:c>
+      <x:c r="C49" s="2">
+        <x:v>44694.5604166667</x:v>
+      </x:c>
+      <x:c r="D49" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E49" s="10" t="s"/>
+      <x:c r="F49" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G49" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H49" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I49" s="10" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="J49" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K49" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L49" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M49" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N49" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O49" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P49" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" hidden="0">
+      <x:c r="A50">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B50" s="2">
+        <x:v>44694.5768402778</x:v>
+      </x:c>
+      <x:c r="C50" s="2">
+        <x:v>44694.5777893519</x:v>
+      </x:c>
+      <x:c r="D50" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E50" s="10" t="s"/>
+      <x:c r="F50" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G50" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H50" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I50" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J50" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K50" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L50" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M50" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N50" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O50" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P50" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" hidden="0">
+      <x:c r="A51">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B51" s="2">
+        <x:v>44694.5933217593</x:v>
+      </x:c>
+      <x:c r="C51" s="2">
+        <x:v>44694.5939814815</x:v>
+      </x:c>
+      <x:c r="D51" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E51" s="10" t="s"/>
+      <x:c r="F51" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G51" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H51" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I51" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J51" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K51" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L51" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="M51" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N51" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O51" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P51" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" hidden="0">
+      <x:c r="A52">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B52" s="2">
+        <x:v>44694.5988657407</x:v>
+      </x:c>
+      <x:c r="C52" s="2">
+        <x:v>44694.599375</x:v>
+      </x:c>
+      <x:c r="D52" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E52" s="10" t="s"/>
+      <x:c r="F52" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G52" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H52" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I52" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J52" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K52" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L52" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M52" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N52" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O52" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P52" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" hidden="0">
+      <x:c r="A53">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B53" s="2">
+        <x:v>44694.6030555556</x:v>
+      </x:c>
+      <x:c r="C53" s="2">
+        <x:v>44694.6038773148</x:v>
+      </x:c>
+      <x:c r="D53" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E53" s="10" t="s"/>
+      <x:c r="F53" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G53" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H53" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I53" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J53" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K53" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L53" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M53" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N53" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O53" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P53" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" hidden="0">
+      <x:c r="A54">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B54" s="2">
+        <x:v>44694.6081828704</x:v>
+      </x:c>
+      <x:c r="C54" s="2">
+        <x:v>44694.6085648148</x:v>
+      </x:c>
+      <x:c r="D54" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E54" s="10" t="s"/>
+      <x:c r="F54" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G54" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H54" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I54" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J54" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K54" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L54" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M54" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N54" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O54" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P54" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" hidden="0">
+      <x:c r="A55">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B55" s="2">
+        <x:v>44694.6113888889</x:v>
+      </x:c>
+      <x:c r="C55" s="2">
+        <x:v>44694.6120601852</x:v>
+      </x:c>
+      <x:c r="D55" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E55" s="10" t="s"/>
+      <x:c r="F55" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G55" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H55" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I55" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J55" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K55" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L55" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M55" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="N55" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O55" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P55" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" hidden="0">
+      <x:c r="A56">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B56" s="2">
+        <x:v>44694.6229166667</x:v>
+      </x:c>
+      <x:c r="C56" s="2">
+        <x:v>44694.6236689815</x:v>
+      </x:c>
+      <x:c r="D56" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E56" s="10" t="s"/>
+      <x:c r="F56" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G56" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H56" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I56" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J56" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K56" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L56" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M56" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="N56" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="O56" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="P56" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" hidden="0">
+      <x:c r="A57">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B57" s="2">
+        <x:v>44694.7706365741</x:v>
+      </x:c>
+      <x:c r="C57" s="2">
+        <x:v>44694.7710416667</x:v>
+      </x:c>
+      <x:c r="D57" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E57" s="10" t="s"/>
+      <x:c r="F57" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G57" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H57" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I57" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J57" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="K57" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L57" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="M57" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N57" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O57" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P57" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" hidden="0">
+      <x:c r="A58">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B58" s="2">
+        <x:v>44694.7725578704</x:v>
+      </x:c>
+      <x:c r="C58" s="2">
+        <x:v>44694.7729398148</x:v>
+      </x:c>
+      <x:c r="D58" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E58" s="10" t="s"/>
+      <x:c r="F58" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G58" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H58" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I58" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="J58" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K58" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L58" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M58" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N58" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="O58" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="P58" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" hidden="0">
+      <x:c r="A59">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B59" s="2">
+        <x:v>44695.0338425926</x:v>
+      </x:c>
+      <x:c r="C59" s="2">
+        <x:v>44695.0356828704</x:v>
+      </x:c>
+      <x:c r="D59" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E59" s="10" t="s"/>
+      <x:c r="F59" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G59" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H59" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I59" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J59" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K59" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="L59" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M59" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N59" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="O59" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P59" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" hidden="0">
+      <x:c r="A60">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B60" s="2">
+        <x:v>44695.3435648148</x:v>
+      </x:c>
+      <x:c r="C60" s="2">
+        <x:v>44695.3446064815</x:v>
+      </x:c>
+      <x:c r="D60" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E60" s="10" t="s"/>
+      <x:c r="F60" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G60" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H60" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I60" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J60" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="K60" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L60" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M60" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="N60" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="O60" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P60" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R20a5bec827ac49f9"/>
+    <x:tablePart r:id="R9cf516556ab64d66"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>